<commit_message>
merge=G* & print preview for milt sheet
</commit_message>
<xml_diff>
--- a/xtt_demo/ZXXT_DEMO_022_R.XLSX
+++ b/xtt_demo/ZXXT_DEMO_022_R.XLSX
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20382"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\moldab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moldab\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76B0ED7-A3C3-40B3-B327-EF5D3408188B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20040" windowHeight="5550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20040" windowHeight="5550" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
-    <sheet name="Info" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet3 ;merge=G0" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="Info" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="G_L1_1">'Sheet2'!$G$12</definedName>
@@ -26,12 +28,12 @@
     <definedName name="H_L1_2">'Sheet2'!$H$20</definedName>
     <definedName name="H_L1_3">'Sheet2'!$H$23</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <r>
       <rPr>
@@ -115,6 +117,9 @@
     <t>Lufthansa</t>
   </si>
   <si>
+    <t>Make groups like 'G*' to create order based cell merging</t>
+  </si>
+  <si>
     <t>NEW YORK</t>
   </si>
   <si>
@@ -169,11 +174,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +233,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -639,7 +652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -746,6 +759,7 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -891,6 +905,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -926,6 +957,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1101,13 +1149,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -1127,47 +1175,47 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s"/>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="48" t="s">
+      <c r="C2" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="52"/>
+      <c r="E2" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="49"/>
+      <c r="G2" s="50"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="46" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46" t="s">
+      <c r="D3" s="51"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="47"/>
+      <c r="G3" s="48"/>
     </row>
     <row r="4" customHeight="1" ht="22.5" hidden="1" outlineLevel="1">
       <c r="A4" t="s"/>
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41" t="s">
+      <c r="D4" s="41"/>
+      <c r="E4" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="41"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="15">
         <v>2402</v>
       </c>
@@ -1190,19 +1238,19 @@
       <c r="A5" t="s"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" hidden="1" outlineLevel="2">
@@ -1359,47 +1407,47 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s"/>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="51"/>
-      <c r="E14" s="44" t="s">
+      <c r="C14" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="52"/>
+      <c r="E14" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="49"/>
+      <c r="G14" s="50"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="46" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="46" t="s">
+      <c r="D15" s="51"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="47"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" customHeight="1" ht="22.5" hidden="1" outlineLevel="1">
       <c r="A16" t="s"/>
       <c r="B16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="40"/>
-      <c r="E16" s="41" t="s">
+      <c r="D16" s="41"/>
+      <c r="E16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="41"/>
+      <c r="F16" s="42"/>
       <c r="G16" s="15">
         <v>0408</v>
       </c>
@@ -1410,7 +1458,7 @@
         <v>14</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L16" s="16" t="s">
         <v>17</v>
@@ -1422,19 +1470,19 @@
       <c r="A17" t="s"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="F17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="18" hidden="1" outlineLevel="2">
@@ -1553,47 +1601,47 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s"/>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="51"/>
-      <c r="E24" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="49"/>
+      <c r="C24" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="52"/>
+      <c r="E24" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="50"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="46" t="s">
+      <c r="B25" s="44"/>
+      <c r="C25" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="47"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="48"/>
     </row>
     <row r="26" customHeight="1" ht="22.5" hidden="1" outlineLevel="1">
       <c r="A26" t="s"/>
       <c r="B26" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="40"/>
-      <c r="E26" s="41" t="s">
+      <c r="D26" s="41"/>
+      <c r="E26" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="41"/>
+      <c r="F26" s="42"/>
       <c r="G26" s="15">
         <v>0400</v>
       </c>
@@ -1604,10 +1652,10 @@
         <v>14</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
@@ -1616,19 +1664,19 @@
       <c r="A27" t="s"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="F27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="28" hidden="1" outlineLevel="2">
@@ -1686,7 +1734,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1710,12 +1758,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s"/>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" customHeight="1" ht="47.25">
       <c r="B2" s="17" t="s">
@@ -1728,7 +1776,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>4</v>
@@ -1737,20 +1785,20 @@
         <v>3</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s"/>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
       <c r="J3" s="16" t="s">
         <v>14</v>
       </c>
@@ -1958,13 +2006,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s"/>
-      <c r="B12" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
+      <c r="B12" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
       <c r="G12" s="20">
         <v>3800</v>
       </c>
@@ -1980,15 +2028,15 @@
     </row>
     <row r="13">
       <c r="A13" t="s"/>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
       <c r="J13" s="16" t="s">
         <v>14</v>
       </c>
@@ -1999,7 +2047,7 @@
         <v>6</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" hidden="1" outlineLevel="1">
@@ -2148,13 +2196,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s"/>
-      <c r="B20" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
+      <c r="B20" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
       <c r="G20" s="20">
         <v>2310</v>
       </c>
@@ -2170,26 +2218,26 @@
     </row>
     <row r="21">
       <c r="A21" t="s"/>
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
       <c r="J21" s="16" t="s">
         <v>14</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L21" s="16" t="s">
         <v>6</v>
       </c>
       <c r="M21" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" hidden="1" outlineLevel="1">
@@ -2218,13 +2266,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s"/>
-      <c r="B23" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
+      <c r="B23" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
       <c r="G23" s="20">
         <v>330</v>
       </c>
@@ -2269,15 +2317,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2290,12 +2338,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s"/>
+      <c r="A1" s="40" t="s"/>
       <c r="B1" s="24" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D1" s="25" t="s">
         <v>1</v>
@@ -2304,23 +2352,23 @@
         <v>7</v>
       </c>
       <c r="F1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="I1" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="s"/>
+      <c r="A2" s="40" t="s"/>
       <c r="B2" s="27" t="s">
         <v>6</v>
       </c>
@@ -2350,7 +2398,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s"/>
+      <c r="A3" s="40" t="s"/>
       <c r="B3" s="27" t="s">
         <v>6</v>
       </c>
@@ -2380,7 +2428,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s"/>
+      <c r="A4" s="40" t="s"/>
       <c r="B4" s="27" t="s">
         <v>6</v>
       </c>
@@ -2410,7 +2458,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s"/>
+      <c r="A5" s="40" t="s"/>
       <c r="B5" s="27" t="s">
         <v>6</v>
       </c>
@@ -2440,7 +2488,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s"/>
+      <c r="A6" s="40" t="s"/>
       <c r="B6" s="27" t="s">
         <v>6</v>
       </c>
@@ -2470,7 +2518,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s"/>
+      <c r="A7" s="40" t="s"/>
       <c r="B7" s="27" t="s">
         <v>6</v>
       </c>
@@ -2500,7 +2548,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s"/>
+      <c r="A8" s="40" t="s"/>
       <c r="B8" s="27" t="s">
         <v>6</v>
       </c>
@@ -2530,7 +2578,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s"/>
+      <c r="A9" s="40" t="s"/>
       <c r="B9" s="27" t="s">
         <v>6</v>
       </c>
@@ -2560,12 +2608,12 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s"/>
+      <c r="A10" s="40" t="s"/>
       <c r="B10" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>18</v>
@@ -2590,12 +2638,12 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s"/>
+      <c r="A11" s="40" t="s"/>
       <c r="B11" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="28" t="s">
         <v>18</v>
@@ -2620,12 +2668,12 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s"/>
+      <c r="A12" s="40" t="s"/>
       <c r="B12" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>18</v>
@@ -2650,12 +2698,12 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s"/>
+      <c r="A13" s="40" t="s"/>
       <c r="B13" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" s="28" t="s">
         <v>18</v>
@@ -2680,12 +2728,12 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s"/>
+      <c r="A14" s="40" t="s"/>
       <c r="B14" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>18</v>
@@ -2710,12 +2758,12 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s"/>
+      <c r="A15" s="40" t="s"/>
       <c r="B15" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D15" s="28" t="s">
         <v>18</v>
@@ -2740,12 +2788,12 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s"/>
+      <c r="A16" s="40" t="s"/>
       <c r="B16" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>19</v>
@@ -2770,7 +2818,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s"/>
+      <c r="A17" s="40" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2788,7 +2836,529 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD89C4E9-6DBE-4156-AFFA-D8D8BD2EC852}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T1" sqref="T1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="8.28515625"/>
+    <col customWidth="1" max="2" min="2" width="14"/>
+    <col customWidth="1" max="3" min="3" width="14"/>
+    <col customWidth="1" max="4" min="4" width="14"/>
+    <col customWidth="1" max="6" min="6" width="12.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="40" t="s"/>
+      <c r="B1" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="40" t="s"/>
+      <c r="B2" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="28">
+        <v>2402</v>
+      </c>
+      <c r="F2" s="32">
+        <v>44190.000000000000</v>
+      </c>
+      <c r="G2" s="30">
+        <v>242.00</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="29">
+        <v>475</v>
+      </c>
+      <c r="J2" s="29">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="40" t="s"/>
+      <c r="B3" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="28">
+        <v>2402</v>
+      </c>
+      <c r="F3" s="32">
+        <v>44270.000000000000</v>
+      </c>
+      <c r="G3" s="30">
+        <v>242.00</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="29">
+        <v>475</v>
+      </c>
+      <c r="J3" s="29">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="40" t="s"/>
+      <c r="B4" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="28">
+        <v>2402</v>
+      </c>
+      <c r="F4" s="32">
+        <v>44344.000000000000</v>
+      </c>
+      <c r="G4" s="30">
+        <v>242.00</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="29">
+        <v>475</v>
+      </c>
+      <c r="J4" s="29">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="40" t="s"/>
+      <c r="B5" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="28">
+        <v>2402</v>
+      </c>
+      <c r="F5" s="32">
+        <v>44350.000000000000</v>
+      </c>
+      <c r="G5" s="30">
+        <v>242.00</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="29">
+        <v>475</v>
+      </c>
+      <c r="J5" s="29">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="40" t="s"/>
+      <c r="B6" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="28">
+        <v>2402</v>
+      </c>
+      <c r="F6" s="32">
+        <v>44375.000000000000</v>
+      </c>
+      <c r="G6" s="30">
+        <v>242.00</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="29">
+        <v>475</v>
+      </c>
+      <c r="J6" s="29">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="40" t="s"/>
+      <c r="B7" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="28">
+        <v>2402</v>
+      </c>
+      <c r="F7" s="32">
+        <v>44430.000000000000</v>
+      </c>
+      <c r="G7" s="30">
+        <v>242.00</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="29">
+        <v>475</v>
+      </c>
+      <c r="J7" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="40" t="s"/>
+      <c r="B8" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="28">
+        <v>2402</v>
+      </c>
+      <c r="F8" s="32">
+        <v>44510.000000000000</v>
+      </c>
+      <c r="G8" s="30">
+        <v>242.00</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="29">
+        <v>475</v>
+      </c>
+      <c r="J8" s="29">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="40" t="s"/>
+      <c r="B9" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="28">
+        <v>2402</v>
+      </c>
+      <c r="F9" s="32">
+        <v>44590.000000000000</v>
+      </c>
+      <c r="G9" s="30">
+        <v>242.00</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="29">
+        <v>475</v>
+      </c>
+      <c r="J9" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="40" t="s"/>
+      <c r="B10" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="28">
+        <v>0408</v>
+      </c>
+      <c r="F10" s="32">
+        <v>44190.000000000000</v>
+      </c>
+      <c r="G10" s="30">
+        <v>1061.36</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="29">
+        <v>385</v>
+      </c>
+      <c r="J10" s="29">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="40" t="s"/>
+      <c r="B11" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="28">
+        <v>0408</v>
+      </c>
+      <c r="F11" s="32">
+        <v>44270.000000000000</v>
+      </c>
+      <c r="G11" s="30">
+        <v>1061.36</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="29">
+        <v>385</v>
+      </c>
+      <c r="J11" s="29">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="40" t="s"/>
+      <c r="B12" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="28">
+        <v>0408</v>
+      </c>
+      <c r="F12" s="32">
+        <v>44350.000000000000</v>
+      </c>
+      <c r="G12" s="30">
+        <v>1061.36</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="29">
+        <v>385</v>
+      </c>
+      <c r="J12" s="29">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="40" t="s"/>
+      <c r="B13" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="28">
+        <v>0408</v>
+      </c>
+      <c r="F13" s="32">
+        <v>44430.000000000000</v>
+      </c>
+      <c r="G13" s="30">
+        <v>1061.36</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="29">
+        <v>385</v>
+      </c>
+      <c r="J13" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="40" t="s"/>
+      <c r="B14" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="28">
+        <v>0408</v>
+      </c>
+      <c r="F14" s="32">
+        <v>44510.000000000000</v>
+      </c>
+      <c r="G14" s="30">
+        <v>1061.36</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="29">
+        <v>385</v>
+      </c>
+      <c r="J14" s="29">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="40" t="s"/>
+      <c r="B15" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="28">
+        <v>0408</v>
+      </c>
+      <c r="F15" s="32">
+        <v>44590.000000000000</v>
+      </c>
+      <c r="G15" s="30">
+        <v>1061.36</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="29">
+        <v>385</v>
+      </c>
+      <c r="J15" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="40" t="s"/>
+      <c r="B16" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="28">
+        <v>0400</v>
+      </c>
+      <c r="F16" s="32">
+        <v>44190.000000000000</v>
+      </c>
+      <c r="G16" s="30">
+        <v>666.00</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="29">
+        <v>330</v>
+      </c>
+      <c r="J16" s="29">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="40" t="s"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B2:B16"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="E2:E9"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="E10:E15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2810,12 +3380,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s"/>
+      <c r="A1" s="40" t="s"/>
       <c r="B1" s="24" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D1" s="25" t="s">
         <v>1</v>
@@ -2824,26 +3394,26 @@
         <v>7</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="J1" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="s"/>
+      <c r="A2" s="40" t="s"/>
       <c r="B2" s="37" t="s">
         <v>6</v>
       </c>
@@ -2876,7 +3446,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s"/>
+      <c r="A3" s="40" t="s"/>
       <c r="B3" s="37" t="s">
         <v>6</v>
       </c>
@@ -2909,7 +3479,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s"/>
+      <c r="A4" s="40" t="s"/>
       <c r="B4" s="37" t="s">
         <v>6</v>
       </c>
@@ -2942,7 +3512,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s"/>
+      <c r="A5" s="40" t="s"/>
       <c r="B5" s="37" t="s">
         <v>6</v>
       </c>
@@ -2975,7 +3545,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s"/>
+      <c r="A6" s="40" t="s"/>
       <c r="B6" s="37" t="s">
         <v>6</v>
       </c>
@@ -3008,7 +3578,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s"/>
+      <c r="A7" s="40" t="s"/>
       <c r="B7" s="37" t="s">
         <v>6</v>
       </c>
@@ -3041,7 +3611,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s"/>
+      <c r="A8" s="40" t="s"/>
       <c r="B8" s="37" t="s">
         <v>6</v>
       </c>
@@ -3074,7 +3644,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s"/>
+      <c r="A9" s="40" t="s"/>
       <c r="B9" s="37" t="s">
         <v>6</v>
       </c>
@@ -3107,7 +3677,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s"/>
+      <c r="A10" s="40" t="s"/>
       <c r="B10" s="27" t="s">
         <v>6</v>
       </c>
@@ -3132,12 +3702,12 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s"/>
+      <c r="A11" s="40" t="s"/>
       <c r="B11" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="38" t="s">
         <v>18</v>
@@ -3165,12 +3735,12 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s"/>
+      <c r="A12" s="40" t="s"/>
       <c r="B12" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="38" t="s">
         <v>18</v>
@@ -3198,12 +3768,12 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s"/>
+      <c r="A13" s="40" t="s"/>
       <c r="B13" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" s="38" t="s">
         <v>18</v>
@@ -3231,12 +3801,12 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s"/>
+      <c r="A14" s="40" t="s"/>
       <c r="B14" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" s="38" t="s">
         <v>18</v>
@@ -3264,12 +3834,12 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s"/>
+      <c r="A15" s="40" t="s"/>
       <c r="B15" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D15" s="38" t="s">
         <v>18</v>
@@ -3297,12 +3867,12 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s"/>
+      <c r="A16" s="40" t="s"/>
       <c r="B16" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D16" s="38" t="s">
         <v>18</v>
@@ -3330,12 +3900,12 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s"/>
+      <c r="A17" s="40" t="s"/>
       <c r="B17" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D17" s="28" t="s">
         <v>18</v>
@@ -3355,12 +3925,12 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s"/>
+      <c r="A18" s="40" t="s"/>
       <c r="B18" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D18" s="38" t="s">
         <v>19</v>
@@ -3388,12 +3958,12 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s"/>
+      <c r="A19" s="40" t="s"/>
       <c r="B19" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D19" s="28" t="s">
         <v>19</v>
@@ -3413,7 +3983,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s"/>
+      <c r="A20" s="40" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3429,8 +3999,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3441,29 +4011,29 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
XTT 022 for MS Word
</commit_message>
<xml_diff>
--- a/xtt_demo/ZXXT_DEMO_022_R.XLSX
+++ b/xtt_demo/ZXXT_DEMO_022_R.XLSX
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moldab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\modekz\Desktop\Gaziz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76B0ED7-A3C3-40B3-B327-EF5D3408188B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCDC94D-7FFA-42AC-9606-58CAED429D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20040" windowHeight="5550" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,11 +29,22 @@
     <definedName name="H_L1_3">'Sheet2'!$H$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <r>
       <rPr>
@@ -57,6 +68,34 @@
         <scheme val="minor"/>
       </rPr>
       <t>with white font for specific level!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>On the other hand the 'merge=G*' depends on previous (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>left</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) column </t>
     </r>
   </si>
   <si>
@@ -117,9 +156,6 @@
     <t>Lufthansa</t>
   </si>
   <si>
-    <t>Make groups like 'G*' to create order based cell merging</t>
-  </si>
-  <si>
     <t>NEW YORK</t>
   </si>
   <si>
@@ -139,6 +175,9 @@
   </si>
   <si>
     <t>TOKYO</t>
+  </si>
+  <si>
+    <t>The 'merge=X' is greedy &amp; combine all same values to 1 cell</t>
   </si>
   <si>
     <t>To</t>
@@ -652,7 +691,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -810,6 +849,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1159,15 +1201,15 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="8.28515625"/>
+    <col customWidth="1" max="1" min="1" width="8.33203125"/>
     <col customWidth="1" max="2" min="2" width="8"/>
-    <col customWidth="1" max="3" min="3" width="16.140625"/>
-    <col customWidth="1" max="4" min="4" width="16.140625"/>
+    <col customWidth="1" max="3" min="3" width="16.109375"/>
+    <col customWidth="1" max="4" min="4" width="16.109375"/>
     <col customWidth="1" max="5" min="5" width="8"/>
-    <col customWidth="1" max="6" min="6" width="16.140625"/>
-    <col customWidth="1" max="7" min="7" width="16.140625"/>
+    <col customWidth="1" max="6" min="6" width="16.109375"/>
+    <col customWidth="1" max="7" min="7" width="16.109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1176,17 +1218,17 @@
     <row r="2">
       <c r="A2" s="1" t="s"/>
       <c r="B2" s="43" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="52"/>
       <c r="E2" s="45" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" s="49" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" s="50"/>
     </row>
@@ -1194,42 +1236,42 @@
       <c r="A3" s="1" t="s"/>
       <c r="B3" s="44"/>
       <c r="C3" s="47" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="51"/>
       <c r="E3" s="46"/>
       <c r="F3" s="47" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="48"/>
     </row>
     <row r="4" customHeight="1" ht="22.5" hidden="1" outlineLevel="1">
       <c r="A4" t="s"/>
       <c r="B4" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="41"/>
       <c r="E4" s="42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="15">
         <v>2402</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
@@ -1238,184 +1280,184 @@
       <c r="A5" t="s"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" hidden="1" outlineLevel="2">
       <c r="A6" t="s"/>
       <c r="B6" s="9"/>
       <c r="C6" s="14">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="D6" s="10">
         <v>242.00</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6" s="11">
         <v>475</v>
       </c>
       <c r="G6" s="12">
-        <v>457</v>
+        <v>451</v>
       </c>
     </row>
     <row r="7" hidden="1" outlineLevel="2">
       <c r="A7" t="s"/>
       <c r="B7" s="9"/>
       <c r="C7" s="14">
-        <v>44270.000000000000</v>
+        <v>45313.000000000000</v>
       </c>
       <c r="D7" s="10">
         <v>242.00</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F7" s="11">
         <v>475</v>
       </c>
       <c r="G7" s="12">
-        <v>461</v>
+        <v>452</v>
       </c>
     </row>
     <row r="8" hidden="1" outlineLevel="2">
       <c r="A8" t="s"/>
       <c r="B8" s="9"/>
       <c r="C8" s="14">
-        <v>44344.000000000000</v>
+        <v>45393.000000000000</v>
       </c>
       <c r="D8" s="10">
         <v>242.00</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F8" s="11">
         <v>475</v>
       </c>
       <c r="G8" s="12">
-        <v>451</v>
+        <v>461</v>
       </c>
     </row>
     <row r="9" hidden="1" outlineLevel="2">
       <c r="A9" t="s"/>
       <c r="B9" s="9"/>
       <c r="C9" s="14">
-        <v>44350.000000000000</v>
+        <v>45410.000000000000</v>
       </c>
       <c r="D9" s="10">
         <v>242.00</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F9" s="11">
         <v>475</v>
       </c>
       <c r="G9" s="12">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="10" hidden="1" outlineLevel="2">
       <c r="A10" t="s"/>
       <c r="B10" s="9"/>
       <c r="C10" s="14">
-        <v>44375.000000000000</v>
+        <v>45440.000000000000</v>
       </c>
       <c r="D10" s="10">
         <v>242.00</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F10" s="11">
         <v>475</v>
       </c>
       <c r="G10" s="12">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="11" hidden="1" outlineLevel="2">
       <c r="A11" t="s"/>
       <c r="B11" s="9"/>
       <c r="C11" s="14">
-        <v>44430.000000000000</v>
+        <v>45473.000000000000</v>
       </c>
       <c r="D11" s="10">
         <v>242.00</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F11" s="11">
         <v>475</v>
       </c>
       <c r="G11" s="12">
-        <v>3</v>
+        <v>459</v>
       </c>
     </row>
     <row r="12" hidden="1" outlineLevel="2">
       <c r="A12" t="s"/>
       <c r="B12" s="9"/>
       <c r="C12" s="14">
-        <v>44510.000000000000</v>
+        <v>45553.000000000000</v>
       </c>
       <c r="D12" s="10">
         <v>242.00</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F12" s="11">
         <v>475</v>
       </c>
       <c r="G12" s="12">
-        <v>87</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" hidden="1" outlineLevel="2">
       <c r="A13" t="s"/>
       <c r="B13" s="9"/>
       <c r="C13" s="14">
-        <v>44590.000000000000</v>
+        <v>45633.000000000000</v>
       </c>
       <c r="D13" s="10">
         <v>242.00</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F13" s="11">
         <v>475</v>
       </c>
       <c r="G13" s="12">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s"/>
       <c r="B14" s="43" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" s="52"/>
       <c r="E14" s="45" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F14" s="49" t="s">
         <v>27</v>
@@ -1426,42 +1468,42 @@
       <c r="A15" s="1" t="s"/>
       <c r="B15" s="44"/>
       <c r="C15" s="47" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" s="51"/>
       <c r="E15" s="46"/>
       <c r="F15" s="47" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G15" s="48"/>
     </row>
     <row r="16" customHeight="1" ht="22.5" hidden="1" outlineLevel="1">
       <c r="A16" t="s"/>
       <c r="B16" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D16" s="41"/>
       <c r="E16" s="42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F16" s="42"/>
       <c r="G16" s="15">
         <v>0408</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>27</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
@@ -1470,146 +1512,146 @@
       <c r="A17" t="s"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="F17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="18" hidden="1" outlineLevel="2">
       <c r="A18" t="s"/>
       <c r="B18" s="9"/>
       <c r="C18" s="14">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="D18" s="10">
         <v>1061.36</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F18" s="11">
         <v>385</v>
       </c>
       <c r="G18" s="12">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="19" hidden="1" outlineLevel="2">
       <c r="A19" t="s"/>
       <c r="B19" s="9"/>
       <c r="C19" s="14">
-        <v>44270.000000000000</v>
+        <v>45313.000000000000</v>
       </c>
       <c r="D19" s="10">
         <v>1061.36</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F19" s="11">
         <v>385</v>
       </c>
       <c r="G19" s="12">
-        <v>369</v>
+        <v>373</v>
       </c>
     </row>
     <row r="20" hidden="1" outlineLevel="2">
       <c r="A20" t="s"/>
       <c r="B20" s="9"/>
       <c r="C20" s="14">
-        <v>44350.000000000000</v>
+        <v>45393.000000000000</v>
       </c>
       <c r="D20" s="10">
         <v>1061.36</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F20" s="11">
         <v>385</v>
       </c>
       <c r="G20" s="12">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="21" hidden="1" outlineLevel="2">
       <c r="A21" t="s"/>
       <c r="B21" s="9"/>
       <c r="C21" s="14">
-        <v>44430.000000000000</v>
+        <v>45473.000000000000</v>
       </c>
       <c r="D21" s="10">
         <v>1061.36</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F21" s="11">
         <v>385</v>
       </c>
       <c r="G21" s="12">
-        <v>0</v>
+        <v>364</v>
       </c>
     </row>
     <row r="22" hidden="1" outlineLevel="2">
       <c r="A22" t="s"/>
       <c r="B22" s="9"/>
       <c r="C22" s="14">
-        <v>44510.000000000000</v>
+        <v>45553.000000000000</v>
       </c>
       <c r="D22" s="10">
         <v>1061.36</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F22" s="11">
         <v>385</v>
       </c>
       <c r="G22" s="12">
-        <v>123</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" hidden="1" outlineLevel="2">
       <c r="A23" t="s"/>
       <c r="B23" s="9"/>
       <c r="C23" s="14">
-        <v>44590.000000000000</v>
+        <v>45633.000000000000</v>
       </c>
       <c r="D23" s="10">
         <v>1061.36</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F23" s="11">
         <v>385</v>
       </c>
       <c r="G23" s="12">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s"/>
       <c r="B24" s="43" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D24" s="52"/>
       <c r="E24" s="45" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F24" s="49" t="s">
         <v>21</v>
@@ -1620,42 +1662,42 @@
       <c r="A25" s="1" t="s"/>
       <c r="B25" s="44"/>
       <c r="C25" s="47" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D25" s="51"/>
       <c r="E25" s="46"/>
       <c r="F25" s="47" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G25" s="48"/>
     </row>
     <row r="26" customHeight="1" ht="22.5" hidden="1" outlineLevel="1">
       <c r="A26" t="s"/>
       <c r="B26" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" s="41" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D26" s="41"/>
       <c r="E26" s="42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F26" s="42"/>
       <c r="G26" s="15">
         <v>0400</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K26" s="16" t="s">
         <v>21</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
@@ -1664,38 +1706,38 @@
       <c r="A27" t="s"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="F27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="28" hidden="1" outlineLevel="2">
       <c r="A28" t="s"/>
       <c r="B28" s="9"/>
       <c r="C28" s="14">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="D28" s="10">
         <v>666.00</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F28" s="11">
         <v>330</v>
       </c>
       <c r="G28" s="12">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="29">
@@ -1744,16 +1786,16 @@
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="8.28515625"/>
-    <col customWidth="1" max="2" min="2" width="24.28515625"/>
-    <col customWidth="1" max="3" min="3" width="11.140625"/>
-    <col customWidth="1" max="4" min="4" width="12.140625"/>
-    <col customWidth="1" max="5" min="5" width="12.140625"/>
-    <col customWidth="1" max="6" min="6" width="8.140625"/>
-    <col customWidth="1" max="7" min="7" width="12.140625"/>
-    <col customWidth="1" max="8" min="8" width="12.140625"/>
+    <col customWidth="1" max="1" min="1" width="8.33203125"/>
+    <col customWidth="1" max="2" min="2" width="24.33203125"/>
+    <col customWidth="1" max="3" min="3" width="11.109375"/>
+    <col customWidth="1" max="4" min="4" width="12.109375"/>
+    <col customWidth="1" max="5" min="5" width="12.109375"/>
+    <col customWidth="1" max="6" min="6" width="8.109375"/>
+    <col customWidth="1" max="7" min="7" width="12.109375"/>
+    <col customWidth="1" max="8" min="8" width="12.109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1767,22 +1809,22 @@
     </row>
     <row r="2" customHeight="1" ht="47.25">
       <c r="B2" s="17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>4</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>3</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>22</v>
@@ -1791,7 +1833,7 @@
     <row r="3">
       <c r="A3" t="s"/>
       <c r="B3" s="53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="53"/>
       <c r="D3" s="53"/>
@@ -1800,208 +1842,208 @@
       <c r="G3" s="53"/>
       <c r="H3" s="53"/>
       <c r="J3" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" hidden="1" outlineLevel="1">
       <c r="A4" t="s"/>
       <c r="B4" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="18">
         <v>2402</v>
       </c>
       <c r="D4" s="21">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="E4" s="18">
         <v>242.00</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G4" s="19">
         <v>475</v>
       </c>
       <c r="H4" s="19">
-        <v>457</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5" hidden="1" outlineLevel="1">
       <c r="A5" t="s"/>
       <c r="B5" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="18">
         <v>2402</v>
       </c>
       <c r="D5" s="21">
-        <v>44270.000000000000</v>
+        <v>45313.000000000000</v>
       </c>
       <c r="E5" s="18">
         <v>242.00</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G5" s="19">
         <v>475</v>
       </c>
       <c r="H5" s="19">
-        <v>461</v>
+        <v>452</v>
       </c>
     </row>
     <row r="6" hidden="1" outlineLevel="1">
       <c r="A6" t="s"/>
       <c r="B6" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="18">
         <v>2402</v>
       </c>
       <c r="D6" s="21">
-        <v>44344.000000000000</v>
+        <v>45393.000000000000</v>
       </c>
       <c r="E6" s="18">
         <v>242.00</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G6" s="19">
         <v>475</v>
       </c>
       <c r="H6" s="19">
-        <v>451</v>
+        <v>461</v>
       </c>
     </row>
     <row r="7" hidden="1" outlineLevel="1">
       <c r="A7" t="s"/>
       <c r="B7" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="18">
         <v>2402</v>
       </c>
       <c r="D7" s="21">
-        <v>44350.000000000000</v>
+        <v>45410.000000000000</v>
       </c>
       <c r="E7" s="18">
         <v>242.00</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G7" s="19">
         <v>475</v>
       </c>
       <c r="H7" s="19">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" hidden="1" outlineLevel="1">
       <c r="A8" t="s"/>
       <c r="B8" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" s="18">
         <v>2402</v>
       </c>
       <c r="D8" s="21">
-        <v>44375.000000000000</v>
+        <v>45440.000000000000</v>
       </c>
       <c r="E8" s="18">
         <v>242.00</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G8" s="19">
         <v>475</v>
       </c>
       <c r="H8" s="19">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="9" hidden="1" outlineLevel="1">
       <c r="A9" t="s"/>
       <c r="B9" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="18">
         <v>2402</v>
       </c>
       <c r="D9" s="21">
-        <v>44430.000000000000</v>
+        <v>45473.000000000000</v>
       </c>
       <c r="E9" s="18">
         <v>242.00</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G9" s="19">
         <v>475</v>
       </c>
       <c r="H9" s="19">
-        <v>3</v>
+        <v>459</v>
       </c>
     </row>
     <row r="10" hidden="1" outlineLevel="1">
       <c r="A10" t="s"/>
       <c r="B10" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="18">
         <v>2402</v>
       </c>
       <c r="D10" s="21">
-        <v>44510.000000000000</v>
+        <v>45553.000000000000</v>
       </c>
       <c r="E10" s="18">
         <v>242.00</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G10" s="19">
         <v>475</v>
       </c>
       <c r="H10" s="19">
-        <v>87</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" hidden="1" outlineLevel="1">
       <c r="A11" t="s"/>
       <c r="B11" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" s="18">
         <v>2402</v>
       </c>
       <c r="D11" s="21">
-        <v>44590.000000000000</v>
+        <v>45633.000000000000</v>
       </c>
       <c r="E11" s="18">
         <v>242.00</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G11" s="19">
         <v>475</v>
       </c>
       <c r="H11" s="19">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
@@ -2017,19 +2059,19 @@
         <v>3800</v>
       </c>
       <c r="H12" s="20">
-        <v>2382</v>
+        <v>2965</v>
       </c>
       <c r="J12" s="16">
         <v>3800</v>
       </c>
       <c r="K12" s="16">
-        <v>2382</v>
+        <v>2965</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s"/>
       <c r="B13" s="53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="53"/>
       <c r="D13" s="53"/>
@@ -2038,13 +2080,13 @@
       <c r="G13" s="53"/>
       <c r="H13" s="53"/>
       <c r="J13" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M13" s="16" t="s">
         <v>27</v>
@@ -2053,145 +2095,145 @@
     <row r="14" hidden="1" outlineLevel="1">
       <c r="A14" t="s"/>
       <c r="B14" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="18">
         <v>0408</v>
       </c>
       <c r="D14" s="21">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="E14" s="18">
         <v>1061.36</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G14" s="19">
         <v>385</v>
       </c>
       <c r="H14" s="19">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="15" hidden="1" outlineLevel="1">
       <c r="A15" t="s"/>
       <c r="B15" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" s="18">
         <v>0408</v>
       </c>
       <c r="D15" s="21">
-        <v>44270.000000000000</v>
+        <v>45313.000000000000</v>
       </c>
       <c r="E15" s="18">
         <v>1061.36</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G15" s="19">
         <v>385</v>
       </c>
       <c r="H15" s="19">
-        <v>369</v>
+        <v>373</v>
       </c>
     </row>
     <row r="16" hidden="1" outlineLevel="1">
       <c r="A16" t="s"/>
       <c r="B16" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" s="18">
         <v>0408</v>
       </c>
       <c r="D16" s="21">
-        <v>44350.000000000000</v>
+        <v>45393.000000000000</v>
       </c>
       <c r="E16" s="18">
         <v>1061.36</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G16" s="19">
         <v>385</v>
       </c>
       <c r="H16" s="19">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="17" hidden="1" outlineLevel="1">
       <c r="A17" t="s"/>
       <c r="B17" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" s="18">
         <v>0408</v>
       </c>
       <c r="D17" s="21">
-        <v>44430.000000000000</v>
+        <v>45473.000000000000</v>
       </c>
       <c r="E17" s="18">
         <v>1061.36</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G17" s="19">
         <v>385</v>
       </c>
       <c r="H17" s="19">
-        <v>0</v>
+        <v>364</v>
       </c>
     </row>
     <row r="18" hidden="1" outlineLevel="1">
       <c r="A18" t="s"/>
       <c r="B18" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18" s="18">
         <v>0408</v>
       </c>
       <c r="D18" s="21">
-        <v>44510.000000000000</v>
+        <v>45553.000000000000</v>
       </c>
       <c r="E18" s="18">
         <v>1061.36</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G18" s="19">
         <v>385</v>
       </c>
       <c r="H18" s="19">
-        <v>123</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" hidden="1" outlineLevel="1">
       <c r="A19" t="s"/>
       <c r="B19" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" s="18">
         <v>0408</v>
       </c>
       <c r="D19" s="21">
-        <v>44590.000000000000</v>
+        <v>45633.000000000000</v>
       </c>
       <c r="E19" s="18">
         <v>1061.36</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G19" s="19">
         <v>385</v>
       </c>
       <c r="H19" s="19">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20">
@@ -2207,19 +2249,19 @@
         <v>2310</v>
       </c>
       <c r="H20" s="20">
-        <v>1233</v>
+        <v>1543</v>
       </c>
       <c r="J20" s="16">
         <v>2310</v>
       </c>
       <c r="K20" s="16">
-        <v>1233</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s"/>
       <c r="B21" s="53" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C21" s="53"/>
       <c r="D21" s="53"/>
@@ -2228,13 +2270,13 @@
       <c r="G21" s="53"/>
       <c r="H21" s="53"/>
       <c r="J21" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M21" s="16" t="s">
         <v>21</v>
@@ -2243,25 +2285,25 @@
     <row r="22" hidden="1" outlineLevel="1">
       <c r="A22" t="s"/>
       <c r="B22" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C22" s="18">
         <v>0400</v>
       </c>
       <c r="D22" s="21">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="E22" s="18">
         <v>666.00</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G22" s="19">
         <v>330</v>
       </c>
       <c r="H22" s="19">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="23">
@@ -2277,13 +2319,13 @@
         <v>330</v>
       </c>
       <c r="H23" s="20">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="J23" s="16">
         <v>330</v>
       </c>
       <c r="K23" s="16">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="24">
@@ -2292,7 +2334,7 @@
     <row r="25">
       <c r="A25" t="s"/>
       <c r="B25" s="23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G25" s="22">
         <f>SUM(G_L1_1,G_L1_2,G_L1_3)</f>
@@ -2321,507 +2363,519 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="8.28515625"/>
+    <col customWidth="1" max="1" min="1" width="8.33203125"/>
     <col customWidth="1" max="2" min="2" width="14"/>
     <col customWidth="1" max="3" min="3" width="14"/>
     <col customWidth="1" max="4" min="4" width="14"/>
-    <col customWidth="1" max="6" min="6" width="12.42578125"/>
+    <col customWidth="1" max="6" min="6" width="12.44140625"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="40" t="s"/>
       <c r="B1" s="24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>36</v>
-      </c>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
     </row>
     <row r="2">
       <c r="A2" s="40" t="s"/>
       <c r="B2" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="28">
         <v>2402</v>
       </c>
       <c r="F2" s="32">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="G2" s="30">
         <v>242.00</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I2" s="29">
         <v>475</v>
       </c>
       <c r="J2" s="29">
-        <v>457</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="40" t="s"/>
       <c r="B3" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="28">
         <v>2402</v>
       </c>
       <c r="F3" s="32">
-        <v>44270.000000000000</v>
+        <v>45313.000000000000</v>
       </c>
       <c r="G3" s="30">
         <v>242.00</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I3" s="29">
         <v>475</v>
       </c>
       <c r="J3" s="29">
-        <v>461</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="40" t="s"/>
       <c r="B4" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="28">
         <v>2402</v>
       </c>
       <c r="F4" s="32">
-        <v>44344.000000000000</v>
+        <v>45393.000000000000</v>
       </c>
       <c r="G4" s="30">
         <v>242.00</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4" s="29">
         <v>475</v>
       </c>
       <c r="J4" s="29">
-        <v>451</v>
+        <v>461</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="40" t="s"/>
       <c r="B5" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="28">
         <v>2402</v>
       </c>
       <c r="F5" s="32">
-        <v>44350.000000000000</v>
+        <v>45410.000000000000</v>
       </c>
       <c r="G5" s="30">
         <v>242.00</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I5" s="29">
         <v>475</v>
       </c>
       <c r="J5" s="29">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="40" t="s"/>
       <c r="B6" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="28">
         <v>2402</v>
       </c>
       <c r="F6" s="32">
-        <v>44375.000000000000</v>
+        <v>45440.000000000000</v>
       </c>
       <c r="G6" s="30">
         <v>242.00</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I6" s="29">
         <v>475</v>
       </c>
       <c r="J6" s="29">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="40" t="s"/>
       <c r="B7" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" s="28">
         <v>2402</v>
       </c>
       <c r="F7" s="32">
-        <v>44430.000000000000</v>
+        <v>45473.000000000000</v>
       </c>
       <c r="G7" s="30">
         <v>242.00</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I7" s="29">
         <v>475</v>
       </c>
       <c r="J7" s="29">
-        <v>3</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="40" t="s"/>
       <c r="B8" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" s="28">
         <v>2402</v>
       </c>
       <c r="F8" s="32">
-        <v>44510.000000000000</v>
+        <v>45553.000000000000</v>
       </c>
       <c r="G8" s="30">
         <v>242.00</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I8" s="29">
         <v>475</v>
       </c>
       <c r="J8" s="29">
-        <v>87</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="40" t="s"/>
       <c r="B9" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="28">
         <v>2402</v>
       </c>
       <c r="F9" s="32">
-        <v>44590.000000000000</v>
+        <v>45633.000000000000</v>
       </c>
       <c r="G9" s="30">
         <v>242.00</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I9" s="29">
         <v>475</v>
       </c>
       <c r="J9" s="29">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="40" t="s"/>
       <c r="B10" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" s="28">
         <v>0408</v>
       </c>
       <c r="F10" s="32">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="G10" s="30">
         <v>1061.36</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I10" s="29">
         <v>385</v>
       </c>
       <c r="J10" s="29">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="40" t="s"/>
       <c r="B11" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" s="28">
         <v>0408</v>
       </c>
       <c r="F11" s="32">
-        <v>44270.000000000000</v>
+        <v>45313.000000000000</v>
       </c>
       <c r="G11" s="30">
         <v>1061.36</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I11" s="29">
         <v>385</v>
       </c>
       <c r="J11" s="29">
-        <v>369</v>
+        <v>373</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="40" t="s"/>
       <c r="B12" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="28">
         <v>0408</v>
       </c>
       <c r="F12" s="32">
-        <v>44350.000000000000</v>
+        <v>45393.000000000000</v>
       </c>
       <c r="G12" s="30">
         <v>1061.36</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I12" s="29">
         <v>385</v>
       </c>
       <c r="J12" s="29">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="40" t="s"/>
       <c r="B13" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13" s="28">
         <v>0408</v>
       </c>
       <c r="F13" s="32">
-        <v>44430.000000000000</v>
+        <v>45473.000000000000</v>
       </c>
       <c r="G13" s="30">
         <v>1061.36</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I13" s="29">
         <v>385</v>
       </c>
       <c r="J13" s="29">
-        <v>0</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="40" t="s"/>
       <c r="B14" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14" s="28">
         <v>0408</v>
       </c>
       <c r="F14" s="32">
-        <v>44510.000000000000</v>
+        <v>45553.000000000000</v>
       </c>
       <c r="G14" s="30">
         <v>1061.36</v>
       </c>
       <c r="H14" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I14" s="29">
         <v>385</v>
       </c>
       <c r="J14" s="29">
-        <v>123</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="40" t="s"/>
       <c r="B15" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15" s="28">
         <v>0408</v>
       </c>
       <c r="F15" s="32">
-        <v>44590.000000000000</v>
+        <v>45633.000000000000</v>
       </c>
       <c r="G15" s="30">
         <v>1061.36</v>
       </c>
       <c r="H15" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I15" s="29">
         <v>385</v>
       </c>
       <c r="J15" s="29">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="40" t="s"/>
       <c r="B16" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="27" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E16" s="28">
         <v>0400</v>
       </c>
       <c r="F16" s="32">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="G16" s="30">
         <v>666.00</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I16" s="29">
         <v>330</v>
       </c>
       <c r="J16" s="29">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="40" t="s"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="M1:U1"/>
     <mergeCell ref="B2:B16"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D9"/>
@@ -2844,499 +2898,499 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1" sqref="T1"/>
+      <selection pane="bottomLeft" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="8.28515625"/>
+    <col customWidth="1" max="1" min="1" width="8.33203125"/>
     <col customWidth="1" max="2" min="2" width="14"/>
     <col customWidth="1" max="3" min="3" width="14"/>
     <col customWidth="1" max="4" min="4" width="14"/>
-    <col customWidth="1" max="6" min="6" width="12.42578125"/>
+    <col customWidth="1" max="6" min="6" width="12.44140625"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="40" t="s"/>
       <c r="B1" s="24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="40" t="s"/>
       <c r="B2" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="28">
         <v>2402</v>
       </c>
       <c r="F2" s="32">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="G2" s="30">
         <v>242.00</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I2" s="29">
         <v>475</v>
       </c>
       <c r="J2" s="29">
-        <v>457</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="40" t="s"/>
       <c r="B3" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="28">
         <v>2402</v>
       </c>
       <c r="F3" s="32">
-        <v>44270.000000000000</v>
+        <v>45313.000000000000</v>
       </c>
       <c r="G3" s="30">
         <v>242.00</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I3" s="29">
         <v>475</v>
       </c>
       <c r="J3" s="29">
-        <v>461</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="40" t="s"/>
       <c r="B4" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="28">
         <v>2402</v>
       </c>
       <c r="F4" s="32">
-        <v>44344.000000000000</v>
+        <v>45393.000000000000</v>
       </c>
       <c r="G4" s="30">
         <v>242.00</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4" s="29">
         <v>475</v>
       </c>
       <c r="J4" s="29">
-        <v>451</v>
+        <v>461</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="40" t="s"/>
       <c r="B5" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="28">
         <v>2402</v>
       </c>
       <c r="F5" s="32">
-        <v>44350.000000000000</v>
+        <v>45410.000000000000</v>
       </c>
       <c r="G5" s="30">
         <v>242.00</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I5" s="29">
         <v>475</v>
       </c>
       <c r="J5" s="29">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="40" t="s"/>
       <c r="B6" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="28">
         <v>2402</v>
       </c>
       <c r="F6" s="32">
-        <v>44375.000000000000</v>
+        <v>45440.000000000000</v>
       </c>
       <c r="G6" s="30">
         <v>242.00</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I6" s="29">
         <v>475</v>
       </c>
       <c r="J6" s="29">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="40" t="s"/>
       <c r="B7" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" s="28">
         <v>2402</v>
       </c>
       <c r="F7" s="32">
-        <v>44430.000000000000</v>
+        <v>45473.000000000000</v>
       </c>
       <c r="G7" s="30">
         <v>242.00</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I7" s="29">
         <v>475</v>
       </c>
       <c r="J7" s="29">
-        <v>3</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="40" t="s"/>
       <c r="B8" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" s="28">
         <v>2402</v>
       </c>
       <c r="F8" s="32">
-        <v>44510.000000000000</v>
+        <v>45553.000000000000</v>
       </c>
       <c r="G8" s="30">
         <v>242.00</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I8" s="29">
         <v>475</v>
       </c>
       <c r="J8" s="29">
-        <v>87</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="40" t="s"/>
       <c r="B9" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="28">
         <v>2402</v>
       </c>
       <c r="F9" s="32">
-        <v>44590.000000000000</v>
+        <v>45633.000000000000</v>
       </c>
       <c r="G9" s="30">
         <v>242.00</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I9" s="29">
         <v>475</v>
       </c>
       <c r="J9" s="29">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="40" t="s"/>
       <c r="B10" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" s="28">
         <v>0408</v>
       </c>
       <c r="F10" s="32">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="G10" s="30">
         <v>1061.36</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I10" s="29">
         <v>385</v>
       </c>
       <c r="J10" s="29">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="40" t="s"/>
       <c r="B11" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" s="28">
         <v>0408</v>
       </c>
       <c r="F11" s="32">
-        <v>44270.000000000000</v>
+        <v>45313.000000000000</v>
       </c>
       <c r="G11" s="30">
         <v>1061.36</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I11" s="29">
         <v>385</v>
       </c>
       <c r="J11" s="29">
-        <v>369</v>
+        <v>373</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="40" t="s"/>
       <c r="B12" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="28">
         <v>0408</v>
       </c>
       <c r="F12" s="32">
-        <v>44350.000000000000</v>
+        <v>45393.000000000000</v>
       </c>
       <c r="G12" s="30">
         <v>1061.36</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I12" s="29">
         <v>385</v>
       </c>
       <c r="J12" s="29">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="40" t="s"/>
       <c r="B13" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13" s="28">
         <v>0408</v>
       </c>
       <c r="F13" s="32">
-        <v>44430.000000000000</v>
+        <v>45473.000000000000</v>
       </c>
       <c r="G13" s="30">
         <v>1061.36</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I13" s="29">
         <v>385</v>
       </c>
       <c r="J13" s="29">
-        <v>0</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="40" t="s"/>
       <c r="B14" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14" s="28">
         <v>0408</v>
       </c>
       <c r="F14" s="32">
-        <v>44510.000000000000</v>
+        <v>45553.000000000000</v>
       </c>
       <c r="G14" s="30">
         <v>1061.36</v>
       </c>
       <c r="H14" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I14" s="29">
         <v>385</v>
       </c>
       <c r="J14" s="29">
-        <v>123</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="40" t="s"/>
       <c r="B15" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15" s="28">
         <v>0408</v>
       </c>
       <c r="F15" s="32">
-        <v>44590.000000000000</v>
+        <v>45633.000000000000</v>
       </c>
       <c r="G15" s="30">
         <v>1061.36</v>
       </c>
       <c r="H15" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I15" s="29">
         <v>385</v>
       </c>
       <c r="J15" s="29">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="40" t="s"/>
       <c r="B16" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="27" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E16" s="28">
         <v>0400</v>
       </c>
       <c r="F16" s="32">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="G16" s="30">
         <v>666.00</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I16" s="29">
         <v>330</v>
       </c>
       <c r="J16" s="29">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17">
@@ -3353,7 +3407,7 @@
     <mergeCell ref="E10:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3366,62 +3420,62 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="8.28515625"/>
+    <col customWidth="1" max="1" min="1" width="8.33203125"/>
     <col customWidth="1" max="2" min="2" width="14"/>
     <col customWidth="1" max="3" min="3" width="14"/>
     <col customWidth="1" max="4" min="4" width="14"/>
-    <col customWidth="1" max="6" min="6" width="7.42578125"/>
-    <col customWidth="1" max="7" min="7" width="12.42578125"/>
+    <col customWidth="1" max="6" min="6" width="7.44140625"/>
+    <col customWidth="1" max="7" min="7" width="12.44140625"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="40" t="s"/>
       <c r="B1" s="24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>24</v>
       </c>
       <c r="G1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="J1" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="26" t="s">
         <v>37</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="40" t="s"/>
       <c r="B2" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="38">
         <v>2402</v>
@@ -3430,31 +3484,31 @@
         <v>1</v>
       </c>
       <c r="G2" s="32">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="H2" s="30">
         <v>242.00</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J2" s="29">
         <v>475</v>
       </c>
       <c r="K2" s="29">
-        <v>457</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="40" t="s"/>
       <c r="B3" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="38">
         <v>2402</v>
@@ -3463,31 +3517,31 @@
         <v>2</v>
       </c>
       <c r="G3" s="32">
-        <v>44270.000000000000</v>
+        <v>45313.000000000000</v>
       </c>
       <c r="H3" s="30">
         <v>242.00</v>
       </c>
       <c r="I3" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J3" s="29">
         <v>475</v>
       </c>
       <c r="K3" s="29">
-        <v>461</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="40" t="s"/>
       <c r="B4" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="38">
         <v>2402</v>
@@ -3496,31 +3550,31 @@
         <v>3</v>
       </c>
       <c r="G4" s="32">
-        <v>44344.000000000000</v>
+        <v>45393.000000000000</v>
       </c>
       <c r="H4" s="30">
         <v>242.00</v>
       </c>
       <c r="I4" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J4" s="29">
         <v>475</v>
       </c>
       <c r="K4" s="29">
-        <v>451</v>
+        <v>461</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="40" t="s"/>
       <c r="B5" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="38">
         <v>2402</v>
@@ -3529,31 +3583,31 @@
         <v>4</v>
       </c>
       <c r="G5" s="32">
-        <v>44350.000000000000</v>
+        <v>45410.000000000000</v>
       </c>
       <c r="H5" s="30">
         <v>242.00</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J5" s="29">
         <v>475</v>
       </c>
       <c r="K5" s="29">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="40" t="s"/>
       <c r="B6" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="38">
         <v>2402</v>
@@ -3562,31 +3616,31 @@
         <v>5</v>
       </c>
       <c r="G6" s="32">
-        <v>44375.000000000000</v>
+        <v>45440.000000000000</v>
       </c>
       <c r="H6" s="30">
         <v>242.00</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J6" s="29">
         <v>475</v>
       </c>
       <c r="K6" s="29">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="40" t="s"/>
       <c r="B7" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" s="38">
         <v>2402</v>
@@ -3595,31 +3649,31 @@
         <v>6</v>
       </c>
       <c r="G7" s="32">
-        <v>44430.000000000000</v>
+        <v>45473.000000000000</v>
       </c>
       <c r="H7" s="30">
         <v>242.00</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J7" s="29">
         <v>475</v>
       </c>
       <c r="K7" s="29">
-        <v>3</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="40" t="s"/>
       <c r="B8" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" s="38">
         <v>2402</v>
@@ -3628,31 +3682,31 @@
         <v>7</v>
       </c>
       <c r="G8" s="32">
-        <v>44510.000000000000</v>
+        <v>45553.000000000000</v>
       </c>
       <c r="H8" s="30">
         <v>242.00</v>
       </c>
       <c r="I8" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J8" s="29">
         <v>475</v>
       </c>
       <c r="K8" s="29">
-        <v>87</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="40" t="s"/>
       <c r="B9" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="38">
         <v>2402</v>
@@ -3661,31 +3715,31 @@
         <v>8</v>
       </c>
       <c r="G9" s="32">
-        <v>44590.000000000000</v>
+        <v>45633.000000000000</v>
       </c>
       <c r="H9" s="30">
         <v>242.00</v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J9" s="29">
         <v>475</v>
       </c>
       <c r="K9" s="29">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="40" t="s"/>
       <c r="B10" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="33"/>
@@ -3698,19 +3752,19 @@
         <v>3800</v>
       </c>
       <c r="K10" s="36">
-        <v>2382</v>
+        <v>2965</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="40" t="s"/>
       <c r="B11" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" s="37" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" s="38">
         <v>0408</v>
@@ -3719,31 +3773,31 @@
         <v>1</v>
       </c>
       <c r="G11" s="32">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="H11" s="30">
         <v>1061.36</v>
       </c>
       <c r="I11" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J11" s="29">
         <v>385</v>
       </c>
       <c r="K11" s="29">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="40" t="s"/>
       <c r="B12" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="37" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="38">
         <v>0408</v>
@@ -3752,31 +3806,31 @@
         <v>2</v>
       </c>
       <c r="G12" s="32">
-        <v>44270.000000000000</v>
+        <v>45313.000000000000</v>
       </c>
       <c r="H12" s="30">
         <v>1061.36</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J12" s="29">
         <v>385</v>
       </c>
       <c r="K12" s="29">
-        <v>369</v>
+        <v>373</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="40" t="s"/>
       <c r="B13" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="37" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13" s="38">
         <v>0408</v>
@@ -3785,31 +3839,31 @@
         <v>3</v>
       </c>
       <c r="G13" s="32">
-        <v>44350.000000000000</v>
+        <v>45393.000000000000</v>
       </c>
       <c r="H13" s="30">
         <v>1061.36</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J13" s="29">
         <v>385</v>
       </c>
       <c r="K13" s="29">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="40" t="s"/>
       <c r="B14" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" s="37" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14" s="38">
         <v>0408</v>
@@ -3818,31 +3872,31 @@
         <v>4</v>
       </c>
       <c r="G14" s="32">
-        <v>44430.000000000000</v>
+        <v>45473.000000000000</v>
       </c>
       <c r="H14" s="30">
         <v>1061.36</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J14" s="29">
         <v>385</v>
       </c>
       <c r="K14" s="29">
-        <v>0</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="40" t="s"/>
       <c r="B15" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="37" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15" s="38">
         <v>0408</v>
@@ -3851,31 +3905,31 @@
         <v>5</v>
       </c>
       <c r="G15" s="32">
-        <v>44510.000000000000</v>
+        <v>45553.000000000000</v>
       </c>
       <c r="H15" s="30">
         <v>1061.36</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J15" s="29">
         <v>385</v>
       </c>
       <c r="K15" s="29">
-        <v>123</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="40" t="s"/>
       <c r="B16" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="37" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E16" s="38">
         <v>0408</v>
@@ -3884,31 +3938,31 @@
         <v>6</v>
       </c>
       <c r="G16" s="32">
-        <v>44590.000000000000</v>
+        <v>45633.000000000000</v>
       </c>
       <c r="H16" s="30">
         <v>1061.36</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J16" s="29">
         <v>385</v>
       </c>
       <c r="K16" s="29">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="40" t="s"/>
       <c r="B17" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E17" s="28"/>
       <c r="F17" s="33"/>
@@ -3921,19 +3975,19 @@
         <v>2310</v>
       </c>
       <c r="K17" s="36">
-        <v>1233</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="40" t="s"/>
       <c r="B18" s="37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" s="37" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E18" s="38">
         <v>0400</v>
@@ -3942,31 +3996,31 @@
         <v>1</v>
       </c>
       <c r="G18" s="32">
-        <v>44190.000000000000</v>
+        <v>45233.000000000000</v>
       </c>
       <c r="H18" s="30">
         <v>666.00</v>
       </c>
       <c r="I18" s="31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J18" s="29">
         <v>330</v>
       </c>
       <c r="K18" s="29">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="40" t="s"/>
       <c r="B19" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C19" s="27" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E19" s="28"/>
       <c r="F19" s="33"/>
@@ -3979,7 +4033,7 @@
         <v>330</v>
       </c>
       <c r="K19" s="36">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="20">
@@ -3988,7 +4042,7 @@
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B2:B19"/>
-    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D9"/>
     <mergeCell ref="C11:C17"/>
     <mergeCell ref="D11:D16"/>
@@ -4007,7 +4061,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -4016,17 +4070,17 @@
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>